<commit_message>
Ajoute dépendances frcore 03ceb43a0a9c0552e155f952032be68f8956b1b5
</commit_message>
<xml_diff>
--- a/ANS-170-RC/ig/StructureDefinition-TDEAuditEvent.xlsx
+++ b/ANS-170-RC/ig/StructureDefinition-TDEAuditEvent.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/[code]/StructureDefinition/TDEAuditEvent</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/tde/StructureDefinition/TDEAuditEvent</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-15T13:02:31+00:00</t>
+    <t>2026-01-21T14:10:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Traçabilité des évènements d'objets métiers</t>
+    <t>Profil représentant la trace d'un évènement</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>